<commit_message>
answer map in the track list
</commit_message>
<xml_diff>
--- a/dat/Temple list.xlsx
+++ b/dat/Temple list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>LKNUTSON</t>
   </si>
@@ -105,33 +105,6 @@
     <t>track008.mp3</t>
   </si>
   <si>
-    <t>track009.mp3</t>
-  </si>
-  <si>
-    <t>track010.mp3</t>
-  </si>
-  <si>
-    <t>track016.mp3</t>
-  </si>
-  <si>
-    <t>track017.mp3</t>
-  </si>
-  <si>
-    <t>track013.mp3</t>
-  </si>
-  <si>
-    <t>track015.mp3</t>
-  </si>
-  <si>
-    <t>track011.mp3</t>
-  </si>
-  <si>
-    <t>track012.mp3</t>
-  </si>
-  <si>
-    <t>track014.mp3</t>
-  </si>
-  <si>
     <t>track000.mp3</t>
   </si>
   <si>
@@ -219,9 +192,6 @@
     <t>Voice Track Name</t>
   </si>
   <si>
-    <t>Region Track Name</t>
-  </si>
-  <si>
     <t>Old</t>
   </si>
   <si>
@@ -267,40 +237,7 @@
     <t>tracym</t>
   </si>
   <si>
-    <t>arprior</t>
-  </si>
-  <si>
-    <t>chicago</t>
-  </si>
-  <si>
-    <t>lubbock</t>
-  </si>
-  <si>
-    <t>pitt</t>
-  </si>
-  <si>
-    <t>prov</t>
-  </si>
-  <si>
-    <t>spokane</t>
-  </si>
-  <si>
-    <t>nyc</t>
-  </si>
-  <si>
-    <t>birm</t>
-  </si>
-  <si>
-    <t>detroit</t>
-  </si>
-  <si>
-    <t>phila_ir</t>
-  </si>
-  <si>
-    <t>phila_bl</t>
-  </si>
-  <si>
-    <t>phila_it</t>
+    <t>Button</t>
   </si>
 </sst>
 </file>
@@ -316,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,12 +275,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,13 +316,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,28 +333,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -778,483 +699,427 @@
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="3">
-        <f>LEN(F3)</f>
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="3">
+        <f>LEN(G3)</f>
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3" s="4">
-        <f>LEN(I3)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="3">
+        <f>LEN(G4)</f>
+        <v>8</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="3">
+        <f>LEN(G5)</f>
+        <v>8</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" ref="G4:G14" si="0">LEN(F4)</f>
+      <c r="C6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="3">
+        <f>LEN(G6)</f>
+        <v>7</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="2">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="3">
+        <f>LEN(G7)</f>
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="3">
+        <f>LEN(G8)</f>
+        <v>6</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="3">
+        <f>LEN(G9)</f>
+        <v>5</v>
+      </c>
+      <c r="I9" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J4" s="4">
-        <f t="shared" ref="J4:J14" si="1">LEN(I4)</f>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="3">
+        <f>LEN(G10)</f>
+        <v>6</v>
+      </c>
+      <c r="I10" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" s="4">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="3">
+        <f>LEN(G11)</f>
+        <v>6</v>
+      </c>
+      <c r="I11" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="3">
-        <f t="shared" si="0"/>
+      <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="3">
+        <f>LEN(G12)</f>
         <v>6</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I12" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="0"/>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="3">
+        <f>LEN(G13)</f>
         <v>6</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="1"/>
+      <c r="I13" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="3">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="3">
+        <f>LEN(G14)</f>
         <v>6</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+      <c r="I14" s="10">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B10">
-    <sortCondition ref="A1"/>
+  <sortState ref="A3:I14">
+    <sortCondition ref="I3"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="C1:D1"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>